<commit_message>
Added C4-C6 to excel
</commit_message>
<xml_diff>
--- a/Control/Controller_gains.xlsx
+++ b/Control/Controller_gains.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mathieu Pellé\Documents\EWEM\S3\LAC\46320_LAC\A3\HAWC_control\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mathieu Pellé\Documents\GitHub\LAC_RotorDesign\Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{94067B66-ED61-432A-B45C-4B763B065927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{148027C2-5788-4A5C-A38E-930CECF0A773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14976" yWindow="2352" windowWidth="11520" windowHeight="12960" xr2:uid="{179E8614-4D99-4493-9CAD-CD59BF548B1F}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12960" xr2:uid="{179E8614-4D99-4493-9CAD-CD59BF548B1F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -83,7 +83,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000E+00"/>
+    <numFmt numFmtId="164" formatCode="0.0000E+00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -131,7 +131,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -553,15 +553,69 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
+      <c r="B5" s="2">
+        <v>20411500</v>
+      </c>
+      <c r="C5" s="2">
+        <v>111389000</v>
+      </c>
+      <c r="D5" s="2">
+        <v>24995500</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2.5749</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.57780699999999996</v>
+      </c>
+      <c r="G5" s="2">
+        <v>4.31691</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
+      <c r="B6" s="2">
+        <v>20411500</v>
+      </c>
+      <c r="C6" s="2">
+        <v>22277700</v>
+      </c>
+      <c r="D6" s="2">
+        <v>999822</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.51497999999999999</v>
+      </c>
+      <c r="F6" s="2">
+        <v>2.3112299999999999E-2</v>
+      </c>
+      <c r="G6" s="2">
+        <v>4.31691</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>20411500</v>
+      </c>
+      <c r="C7" s="2">
+        <v>222777000</v>
+      </c>
+      <c r="D7" s="2">
+        <v>99982200</v>
+      </c>
+      <c r="E7" s="2">
+        <v>5.1497999999999999</v>
+      </c>
+      <c r="F7" s="2">
+        <v>2.3112300000000001</v>
+      </c>
+      <c r="G7" s="2">
+        <v>4.31691</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>